<commit_message>
Updated Diagrams and Data
Updated
</commit_message>
<xml_diff>
--- a/Jack Skellington/Data.xlsx
+++ b/Jack Skellington/Data.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alkal_000\Documents\Halloween\Halloween\Jack Skellington\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="405" windowWidth="20835" windowHeight="11790" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="9312" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Size &amp; Lengths" sheetId="1" r:id="rId1"/>
     <sheet name="BOM" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
-  <si>
-    <t>0.63"</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Neck</t>
   </si>
@@ -32,12 +34,6 @@
     <t>Forearm</t>
   </si>
   <si>
-    <t>Height</t>
-  </si>
-  <si>
-    <t>Width</t>
-  </si>
-  <si>
     <t>Head</t>
   </si>
   <si>
@@ -99,13 +95,25 @@
   </si>
   <si>
     <t>Shipping</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Foam for Head</t>
+  </si>
+  <si>
+    <t>http://www.homedepot.com/p/Project-Panels-2-ft-x-2-ft-Project-Panel-PP1/203553730</t>
+  </si>
+  <si>
+    <t>tax</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +150,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -188,7 +204,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -220,9 +236,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -254,6 +271,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -429,231 +447,182 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <f>B1/B6</f>
+        <v>11.570247933884298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.77</v>
+      </c>
+      <c r="C4">
+        <f>$B$2*B4*H4</f>
+        <v>10.181818181818185</v>
+      </c>
+      <c r="F4">
+        <v>5.39</v>
+      </c>
+      <c r="G4">
+        <v>6.16</v>
+      </c>
+      <c r="H4">
+        <f>G4/F4</f>
+        <v>1.142857142857143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>7.26</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C5:C15" si="0">$B$2*B6</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0.33</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>3.8181818181818183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1.73</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>20.016528925619834</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>0.83</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>9.6033057851239665</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>0.37</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>4.2809917355371905</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>0.39</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>4.5123966942148765</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>1.44</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>16.66115702479339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>1.53</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>17.702479338842977</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>9</v>
-      </c>
-      <c r="B2">
-        <f>B1/D6</f>
-        <v>13.614262560777957</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0.63</v>
-      </c>
-      <c r="E4">
-        <f>D4*$B$2</f>
-        <v>8.5769854132901138</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <f t="shared" ref="E5:E15" si="0">D5*$B$2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>6.17</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <f t="shared" ref="D6:D13" si="1">(SQRT((B6*B6)+(C6*C6)))</f>
-        <v>6.17</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>0.15</v>
-      </c>
-      <c r="C7">
-        <v>0.02</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="1"/>
-        <v>0.15132745950421556</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>2.0602117663458843</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>0.4</v>
-      </c>
-      <c r="C8">
-        <v>1.66</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="1"/>
-        <v>1.7075128110793196</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>23.246527735925905</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9">
-        <f>D8/3</f>
-        <v>0.56917093702643984</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>7.7488425786419688</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10">
-        <f>D8/3</f>
-        <v>0.56917093702643984</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>7.7488425786419688</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11">
-        <f>D8/3</f>
-        <v>0.56917093702643984</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>7.7488425786419688</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12">
-        <f>D13+D14</f>
-        <v>2.8120455188349989</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>38.283926026278749</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>0.13</v>
-      </c>
-      <c r="C13">
-        <v>1.4</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="1"/>
-        <v>1.4060227594174994</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>19.141963013139375</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>0.13</v>
-      </c>
-      <c r="C14">
-        <v>1.4</v>
-      </c>
-      <c r="D14">
-        <f>(SQRT((B14*B14)+(C14*C14)))</f>
-        <v>1.4060227594174994</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>19.141963013139375</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>12</v>
       </c>
       <c r="B15">
         <v>3.76</v>
       </c>
       <c r="C15">
-        <v>0.85</v>
-      </c>
-      <c r="D15">
-        <f>(SQRT((B15*B15)+(C15*C15)))</f>
-        <v>3.854880024073382</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>52.481348788033074</v>
+        <f t="shared" si="0"/>
+        <v>43.504132231404959</v>
       </c>
     </row>
   </sheetData>
@@ -662,52 +631,55 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>6.46</v>
@@ -720,9 +692,9 @@
         <v>25.84</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>17.5</v>
@@ -737,9 +709,31 @@
       <c r="G4">
         <v>6</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <f>F4+G4</f>
         <v>58.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>5.48</v>
+      </c>
+      <c r="E5">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <f>D5*E5</f>
+        <v>60.28</v>
+      </c>
+      <c r="H5">
+        <f>F5*1.09</f>
+        <v>65.705200000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>